<commit_message>
Verificación de indicaciones reunión 28-07-2015
Se verificó el guion entregado de MA_07_02_CO según indicaciones de
Lizzie en la reunión del 28-07-2015
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion02/Escaleta MA_07_02_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion02/Escaleta MA_07_02_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repositorio_MA_07\MA_07_02_CO\MA_07_02_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -632,10 +632,35 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+Debe arreglarese para convertir en un M101A
 Antes
 MA_07_02_CO_REC140
 Ahora
 MA_07_02_CO_REC180</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N20" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jesica:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Debe volverse un M101A</t>
         </r>
       </text>
     </comment>
@@ -893,10 +918,35 @@
           </rPr>
           <t xml:space="preserve">
 Este recurso se eliminó en la propuesta del experto pedagógico, se incluye ya que el recurso está elaborado y cumple el propósito de la sección.
+Debe arreglarese para convertir en un M101A
 Antes
 MA_07_02_CO_REC200
 Ahora
 MA_07_02_CO_REC250</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N27" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jesica:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Debe volverse un M101A</t>
         </r>
       </text>
     </comment>
@@ -2509,7 +2559,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2597,6 +2647,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2721,7 +2777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2879,6 +2935,9 @@
     <xf numFmtId="0" fontId="6" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2928,6 +2987,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7522,8 +7584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7552,94 +7614,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="83" t="s">
+      <c r="C1" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="76" t="s">
+      <c r="E1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="74" t="s">
         <v>208</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="69" t="s">
         <v>209</v>
       </c>
-      <c r="I1" s="80" t="s">
+      <c r="I1" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="69" t="s">
         <v>213</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="80" t="s">
         <v>210</v>
       </c>
-      <c r="L1" s="78" t="s">
+      <c r="L1" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="81" t="s">
+      <c r="M1" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="82"/>
-      <c r="O1" s="75" t="s">
+      <c r="N1" s="83"/>
+      <c r="O1" s="76" t="s">
         <v>211</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="68" t="s">
         <v>212</v>
       </c>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="73" t="s">
         <v>131</v>
       </c>
-      <c r="S1" s="70" t="s">
+      <c r="S1" s="71" t="s">
         <v>132</v>
       </c>
-      <c r="T1" s="71" t="s">
+      <c r="T1" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="U1" s="70" t="s">
+      <c r="U1" s="71" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="77"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="78"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="79"/>
       <c r="M2" s="42" t="s">
         <v>135</v>
       </c>
       <c r="N2" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="O2" s="75"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="72"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="70"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="71"/>
     </row>
     <row r="3" spans="1:23" s="57" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
@@ -8735,7 +8797,7 @@
       <c r="E20" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="85" t="s">
         <v>255</v>
       </c>
       <c r="G20" s="59">
@@ -8757,7 +8819,7 @@
         <v>93</v>
       </c>
       <c r="M20" s="50"/>
-      <c r="N20" s="50" t="s">
+      <c r="N20" s="67" t="s">
         <v>148</v>
       </c>
       <c r="O20" s="32" t="s">
@@ -9168,7 +9230,7 @@
       <c r="E27" s="58" t="s">
         <v>222</v>
       </c>
-      <c r="F27" s="35" t="s">
+      <c r="F27" s="85" t="s">
         <v>309</v>
       </c>
       <c r="G27" s="59">
@@ -9190,7 +9252,7 @@
         <v>93</v>
       </c>
       <c r="M27" s="50"/>
-      <c r="N27" s="50" t="s">
+      <c r="N27" s="67" t="s">
         <v>110</v>
       </c>
       <c r="O27" s="32" t="s">

</xml_diff>